<commit_message>
vault backup: 2025-03-21 10:32:31
</commit_message>
<xml_diff>
--- a/Maths/Statistics/Large_Dataset/Individual Places/jacksonville_15.xlsx
+++ b/Maths/Statistics/Large_Dataset/Individual Places/jacksonville_15.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rgshw-my.sharepoint.com/personal/17abryan_rgshw_com/Documents/6th Form/AS Level/Further Maths/Notes/Statistics/Large_Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97671c4de08f37e/Documents/A-Level Notes/Maths/Statistics/Large_Dataset/Individual Places/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC10489DC9995AD65ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A7ACB96-35D0-4C12-8869-357ACCEBFBBF}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_F25DC773A252ABDACC10489DC9995AD65ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1269004F-7FF7-430A-9624-DE82CF725BD6}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="2925" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -392,12 +392,15 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F185"/>
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -417,7 +420,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="4">
         <v>42125</v>
       </c>
@@ -437,7 +440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="4">
         <v>42126</v>
       </c>
@@ -457,7 +460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="4">
         <v>42127</v>
       </c>
@@ -477,7 +480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="4">
         <v>42128</v>
       </c>
@@ -497,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="4">
         <v>42129</v>
       </c>
@@ -517,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="4">
         <v>42130</v>
       </c>
@@ -537,7 +540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="4">
         <v>42131</v>
       </c>
@@ -557,7 +560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="4">
         <v>42132</v>
       </c>
@@ -577,7 +580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="4">
         <v>42133</v>
       </c>
@@ -597,7 +600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="4">
         <v>42134</v>
       </c>
@@ -617,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="4">
         <v>42135</v>
       </c>
@@ -637,7 +640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="4">
         <v>42136</v>
       </c>
@@ -657,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="4">
         <v>42137</v>
       </c>
@@ -677,7 +680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="4">
         <v>42138</v>
       </c>
@@ -697,7 +700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="4">
         <v>42139</v>
       </c>
@@ -717,7 +720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="4">
         <v>42140</v>
       </c>
@@ -737,7 +740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="4">
         <v>42141</v>
       </c>
@@ -757,7 +760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="4">
         <v>42142</v>
       </c>
@@ -777,7 +780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="4">
         <v>42143</v>
       </c>
@@ -797,7 +800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="4">
         <v>42144</v>
       </c>
@@ -817,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="4">
         <v>42145</v>
       </c>
@@ -837,7 +840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="4">
         <v>42146</v>
       </c>
@@ -857,7 +860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="4">
         <v>42147</v>
       </c>
@@ -877,7 +880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="4">
         <v>42148</v>
       </c>
@@ -897,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="4">
         <v>42149</v>
       </c>
@@ -917,7 +920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="4">
         <v>42150</v>
       </c>
@@ -937,7 +940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="4">
         <v>42151</v>
       </c>
@@ -957,7 +960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="4">
         <v>42152</v>
       </c>
@@ -977,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="4">
         <v>42153</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="4">
         <v>42154</v>
       </c>
@@ -1017,7 +1020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="4">
         <v>42155</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="4">
         <v>42156</v>
       </c>
@@ -1057,7 +1060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="4">
         <v>42157</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="4">
         <v>42158</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="4">
         <v>42159</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="4">
         <v>42160</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="4">
         <v>42161</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="4">
         <v>42162</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="4">
         <v>42163</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="4">
         <v>42164</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="4">
         <v>42165</v>
       </c>
@@ -1237,7 +1240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="4">
         <v>42166</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="4">
         <v>42167</v>
       </c>
@@ -1277,7 +1280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="4">
         <v>42168</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="4">
         <v>42169</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="4">
         <v>42170</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="4">
         <v>42171</v>
       </c>
@@ -1357,7 +1360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="4">
         <v>42172</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="4">
         <v>42173</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="4">
         <v>42174</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="4">
         <v>42175</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="4">
         <v>42176</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="4">
         <v>42177</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="4">
         <v>42178</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="4">
         <v>42179</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="4">
         <v>42180</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="4">
         <v>42181</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="4">
         <v>42182</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="4">
         <v>42183</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="4">
         <v>42184</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4">
         <v>42185</v>
       </c>
@@ -1637,7 +1640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="4">
         <v>42186</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="4">
         <v>42187</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="4">
         <v>42188</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="4">
         <v>42189</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="4">
         <v>42190</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="4">
         <v>42191</v>
       </c>
@@ -1757,7 +1760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="4">
         <v>42192</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="4">
         <v>42193</v>
       </c>
@@ -1797,7 +1800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="4">
         <v>42194</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="4">
         <v>42195</v>
       </c>
@@ -1837,7 +1840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="4">
         <v>42196</v>
       </c>
@@ -1857,7 +1860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="4">
         <v>42197</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="4">
         <v>42198</v>
       </c>
@@ -1897,7 +1900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="4">
         <v>42199</v>
       </c>
@@ -1917,7 +1920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="4">
         <v>42200</v>
       </c>
@@ -1937,7 +1940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="4">
         <v>42201</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="4">
         <v>42202</v>
       </c>
@@ -1977,7 +1980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="4">
         <v>42203</v>
       </c>
@@ -1997,7 +2000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="4">
         <v>42204</v>
       </c>
@@ -2017,7 +2020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="4">
         <v>42205</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="4">
         <v>42206</v>
       </c>
@@ -2057,7 +2060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="4">
         <v>42207</v>
       </c>
@@ -2077,7 +2080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="4">
         <v>42208</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="4">
         <v>42209</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="4">
         <v>42210</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="4">
         <v>42211</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="4">
         <v>42212</v>
       </c>
@@ -2177,7 +2180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="4">
         <v>42213</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="4">
         <v>42214</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="4">
         <v>42215</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="4">
         <v>42216</v>
       </c>
@@ -2257,7 +2260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="4">
         <v>42217</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="4">
         <v>42218</v>
       </c>
@@ -2297,7 +2300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="4">
         <v>42219</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="4">
         <v>42220</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" s="4">
         <v>42221</v>
       </c>
@@ -2357,7 +2360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" s="4">
         <v>42222</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" s="4">
         <v>42223</v>
       </c>
@@ -2397,7 +2400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" s="4">
         <v>42224</v>
       </c>
@@ -2417,7 +2420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" s="4">
         <v>42225</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" s="4">
         <v>42226</v>
       </c>
@@ -2457,7 +2460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" s="4">
         <v>42227</v>
       </c>
@@ -2477,7 +2480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" s="4">
         <v>42228</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" s="4">
         <v>42229</v>
       </c>
@@ -2517,7 +2520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" s="4">
         <v>42230</v>
       </c>
@@ -2537,7 +2540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" s="4">
         <v>42231</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" s="4">
         <v>42232</v>
       </c>
@@ -2577,7 +2580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" s="4">
         <v>42233</v>
       </c>
@@ -2597,7 +2600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" s="4">
         <v>42234</v>
       </c>
@@ -2617,7 +2620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" s="4">
         <v>42235</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" s="4">
         <v>42236</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" s="4">
         <v>42237</v>
       </c>
@@ -2677,7 +2680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" s="4">
         <v>42238</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" s="4">
         <v>42239</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" s="4">
         <v>42240</v>
       </c>
@@ -2737,7 +2740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" s="4">
         <v>42241</v>
       </c>
@@ -2757,7 +2760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" s="4">
         <v>42242</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" s="4">
         <v>42243</v>
       </c>
@@ -2797,7 +2800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" s="4">
         <v>42244</v>
       </c>
@@ -2817,7 +2820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" s="4">
         <v>42245</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" s="4">
         <v>42246</v>
       </c>
@@ -2857,7 +2860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" s="4">
         <v>42247</v>
       </c>
@@ -2877,7 +2880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" s="4">
         <v>42248</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" s="4">
         <v>42249</v>
       </c>
@@ -2917,7 +2920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" s="4">
         <v>42250</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" s="4">
         <v>42251</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" s="4">
         <v>42252</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" s="4">
         <v>42253</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" s="4">
         <v>42254</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" s="4">
         <v>42255</v>
       </c>
@@ -3037,7 +3040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" s="4">
         <v>42256</v>
       </c>
@@ -3057,7 +3060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" s="4">
         <v>42257</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" s="4">
         <v>42258</v>
       </c>
@@ -3097,7 +3100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" s="4">
         <v>42259</v>
       </c>
@@ -3117,7 +3120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" s="4">
         <v>42260</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" s="4">
         <v>42261</v>
       </c>
@@ -3157,7 +3160,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" s="4">
         <v>42262</v>
       </c>
@@ -3177,7 +3180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" s="4">
         <v>42263</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" s="4">
         <v>42264</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" s="4">
         <v>42265</v>
       </c>
@@ -3237,7 +3240,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" s="4">
         <v>42266</v>
       </c>
@@ -3257,7 +3260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" s="4">
         <v>42267</v>
       </c>
@@ -3277,7 +3280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" s="4">
         <v>42268</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" s="4">
         <v>42269</v>
       </c>
@@ -3317,7 +3320,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" s="4">
         <v>42270</v>
       </c>
@@ -3337,7 +3340,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" s="4">
         <v>42271</v>
       </c>
@@ -3357,7 +3360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" s="4">
         <v>42272</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" s="4">
         <v>42273</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" s="4">
         <v>42274</v>
       </c>
@@ -3417,7 +3420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" s="4">
         <v>42275</v>
       </c>
@@ -3437,7 +3440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" s="4">
         <v>42276</v>
       </c>
@@ -3457,7 +3460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" s="4">
         <v>42277</v>
       </c>
@@ -3477,7 +3480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" s="4">
         <v>42278</v>
       </c>
@@ -3497,7 +3500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" s="4">
         <v>42279</v>
       </c>
@@ -3517,7 +3520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" s="4">
         <v>42280</v>
       </c>
@@ -3537,7 +3540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" s="4">
         <v>42281</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" s="4">
         <v>42282</v>
       </c>
@@ -3577,7 +3580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" s="4">
         <v>42283</v>
       </c>
@@ -3597,7 +3600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" s="4">
         <v>42284</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" s="4">
         <v>42285</v>
       </c>
@@ -3637,7 +3640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" s="4">
         <v>42286</v>
       </c>
@@ -3657,7 +3660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" s="4">
         <v>42287</v>
       </c>
@@ -3677,7 +3680,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" s="4">
         <v>42288</v>
       </c>
@@ -3697,7 +3700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" s="4">
         <v>42289</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" s="4">
         <v>42290</v>
       </c>
@@ -3737,7 +3740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" s="4">
         <v>42291</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169" s="4">
         <v>42292</v>
       </c>
@@ -3777,7 +3780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170" s="4">
         <v>42293</v>
       </c>
@@ -3797,7 +3800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171" s="4">
         <v>42294</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172" s="4">
         <v>42295</v>
       </c>
@@ -3837,7 +3840,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173" s="4">
         <v>42296</v>
       </c>
@@ -3857,7 +3860,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174" s="4">
         <v>42297</v>
       </c>
@@ -3877,7 +3880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175" s="4">
         <v>42298</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176" s="4">
         <v>42299</v>
       </c>
@@ -3917,7 +3920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A177" s="4">
         <v>42300</v>
       </c>
@@ -3937,7 +3940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A178" s="4">
         <v>42301</v>
       </c>
@@ -3957,7 +3960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A179" s="4">
         <v>42302</v>
       </c>
@@ -3977,7 +3980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A180" s="4">
         <v>42303</v>
       </c>
@@ -3997,7 +4000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A181" s="4">
         <v>42304</v>
       </c>
@@ -4017,7 +4020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A182" s="4">
         <v>42305</v>
       </c>
@@ -4037,7 +4040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A183" s="4">
         <v>42306</v>
       </c>
@@ -4057,7 +4060,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A184" s="4">
         <v>42307</v>
       </c>
@@ -4077,7 +4080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A185" s="4">
         <v>42308</v>
       </c>

</xml_diff>